<commit_message>
worked on word len menas
</commit_message>
<xml_diff>
--- a/lit/reading_list.xlsx
+++ b/lit/reading_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\debor\masterThesis\lit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC0B5303-9BAE-492C-B184-C822DA534ADE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EC807B6-A292-4F58-9B5F-2412A670B09C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{FAF275AB-D4AD-4F50-96C0-D7F748AA45A3}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{FAF275AB-D4AD-4F50-96C0-D7F748AA45A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="64">
   <si>
     <t>title</t>
   </si>
@@ -256,6 +256,18 @@
   </si>
   <si>
     <t>G2P for quite many languages</t>
+  </si>
+  <si>
+    <t>http://citeseerx.ist.psu.edu/viewdoc/download;jsessionid=308DCC909EF2E6D930D20779A49CEC98?doi=10.1.1.48.9845&amp;rep=rep1&amp;type=pdf</t>
+  </si>
+  <si>
+    <t>https://aclanthology.org/N15-1056.pdf</t>
+  </si>
+  <si>
+    <t>https://aclanthology.org/2021.sigtyp-1.1.pdf</t>
+  </si>
+  <si>
+    <t>https://link.springer.com/article/10.1007/s11145-017-9741-5</t>
   </si>
 </sst>
 </file>
@@ -279,20 +291,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -304,11 +320,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -318,11 +335,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="3">
+    <cellStyle name="Gut" xfId="2" builtinId="26"/>
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -337,8 +360,62 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>120650</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1025" name="AutoShape 1">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5860FB8F-2A6B-4B62-BE7B-4571FF017731}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="2863850" y="18745200"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -634,22 +711,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9A94189-D696-4502-A404-7F70B0E07ED0}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.46484375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="17.53125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="89.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="8.265625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="23.453125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="17.54296875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="12.6328125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="89.6328125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.26953125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -672,7 +749,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="142.5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" ht="145" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>20</v>
       </c>
@@ -692,7 +769,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="185.65" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" ht="185.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>26</v>
       </c>
@@ -712,7 +789,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="156.75" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" ht="203" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>32</v>
       </c>
@@ -732,27 +809,27 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:7" s="8" customFormat="1" ht="87" x14ac:dyDescent="0.35">
+      <c r="A5" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="142.5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>44</v>
       </c>
@@ -769,7 +846,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="213.75" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" ht="232" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>52</v>
       </c>
@@ -789,7 +866,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="270.75" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" ht="304.5" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>56</v>
       </c>
@@ -809,7 +886,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C9" s="3" t="s">
         <v>30</v>
       </c>
@@ -820,7 +897,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C10" s="3" t="s">
         <v>9</v>
       </c>
@@ -831,7 +908,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C11" s="3" t="s">
         <v>10</v>
       </c>
@@ -842,7 +919,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>45</v>
       </c>
@@ -856,7 +933,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>46</v>
       </c>
@@ -870,7 +947,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>48</v>
       </c>
@@ -884,7 +961,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C15" s="3" t="s">
         <v>17</v>
       </c>
@@ -893,6 +970,26 @@
       </c>
       <c r="F15" t="s">
         <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C16" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C17" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C18" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C19" s="5" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -916,8 +1013,12 @@
     <hyperlink ref="C5" r:id="rId12" xr:uid="{74C9CB1C-6862-43D7-8421-53FDB4B80222}"/>
     <hyperlink ref="C13" r:id="rId13" xr:uid="{5A56F792-BE0F-443E-8287-321E8A28F3F0}"/>
     <hyperlink ref="C15" r:id="rId14" xr:uid="{F0DE660A-9093-4981-B9FA-23DA71FFF057}"/>
+    <hyperlink ref="C17" r:id="rId15" xr:uid="{43BF4137-F039-474D-A9C8-989DE72DC26F}"/>
+    <hyperlink ref="C18" r:id="rId16" xr:uid="{B8BEFF98-E9E5-45D2-A251-8EFA7264A617}"/>
+    <hyperlink ref="C19" r:id="rId17" xr:uid="{E3539764-6ED2-4698-B826-79A5EC2841DB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId15"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId18"/>
+  <drawing r:id="rId19"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
char list not in PHOIBLE
</commit_message>
<xml_diff>
--- a/lit/reading_list.xlsx
+++ b/lit/reading_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\debor\masterThesis\lit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EC807B6-A292-4F58-9B5F-2412A670B09C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{400A70BC-DD0F-44BB-8FAA-8ABE073A5861}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{FAF275AB-D4AD-4F50-96C0-D7F748AA45A3}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{FAF275AB-D4AD-4F50-96C0-D7F748AA45A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -171,11 +171,6 @@
       Daelemans, Walter</t>
   </si>
   <si>
-    <t>The modeling of psycholinguistic phenomena, such as word reading, with machine learning techniques requires the featurization of word stimuli into appropriate orthographic and phonological representations. Critically, the choice of features impacts the performance of machine learning algorithms, and can have important ramifications for the conclusions drawn from a model. As such, featurizing words with a variety of feature sets, without having to resort to using different tools is beneficial in terms of development cost. In this work, we
-present wordkit, a python package which allows users to switch between feature sets and featurizers with a uniform API, allowing for rapid prototyping. To the best of our knowledge, this is the first package which integrates a variety of orthographic and phonological featurizers in a single package. The package is fully compatible with scikit-learn, and hence can be integrated into a variety of machine learning pipelines. Furthermore, the package is modular and extensible, allowing for the future integration of a large variety of
-feature sets and featurizers. The package and documentation can be found at github.com/stephantul/wordkit</t>
-  </si>
-  <si>
     <t>Grapheme-to-Phoneme Models for (Almost) Any Language</t>
   </si>
   <si>
@@ -268,6 +263,10 @@
   </si>
   <si>
     <t>https://link.springer.com/article/10.1007/s11145-017-9741-5</t>
+  </si>
+  <si>
+    <t>The modeling of psycholinguistic phenomena, such as word reading, with machine learning techniques requires the featurization of word stimuli into appropriate orthographic and phonological representations. Critically, the choice of features impacts the performance of machine learning algorithms, and can have important ramifications for the conclusions drawn from a model. As such, featurizing words with a variety of feature sets, without having to resort to using different tools is beneficial in terms of development cost. In this work, we present wordkit, a python package which allows users to switch between feature sets and featurizers with a uniform API, allowing for rapid prototyping. To the best of our knowledge, this is the first package which integrates a variety of orthographic and phonological featurizers in a single package. The package is fully compatible with scikit-learn, and hence can be integrated into a variety of machine learning pipelines. Furthermore, the package is modular and extensible, allowing for the future integration of a large variety of
+feature sets and featurizers. The package and documentation can be found at github.com/stephantul/wordkit</t>
   </si>
 </sst>
 </file>
@@ -713,20 +712,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9A94189-D696-4502-A404-7F70B0E07ED0}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.453125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="17.54296875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="12.6328125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="89.6328125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="8.26953125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="23.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="89.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.28515625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -749,7 +748,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="145" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="165" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>20</v>
       </c>
@@ -769,7 +768,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="185.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" ht="213" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>26</v>
       </c>
@@ -789,7 +788,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="203" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" ht="210" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>32</v>
       </c>
@@ -800,7 +799,7 @@
         <v>7</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>35</v>
+        <v>63</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>33</v>
@@ -809,84 +808,84 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="8" customFormat="1" ht="87" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" s="8" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>36</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>37</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>8</v>
       </c>
       <c r="D5" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" s="8" t="s">
         <v>38</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>39</v>
       </c>
       <c r="F5" s="8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" ht="180" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="232" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" ht="255" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>15</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="304.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" ht="330" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C9" s="3" t="s">
         <v>30</v>
       </c>
@@ -897,99 +896,99 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C10" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F10" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C11" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F11" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F12" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F13" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F14" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C15" s="3" t="s">
         <v>17</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F15" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C16" s="5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.35">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C17" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C18" s="5" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C18" s="5" t="s">
+    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C19" s="5" t="s">
         <v>61</v>
-      </c>
-    </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C19" s="5" t="s">
-        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>